<commit_message>
Rewrite sample to use FIMS
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -12,37 +12,80 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data-fims" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lng</t>
-  </si>
-  <si>
-    <t>alt</t>
-  </si>
-  <si>
-    <t>error</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>collectionID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> catalogNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fieldNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diseaseTested</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diseaseStrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sampleMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sampleDisposition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diseaseDetected[TRUE|FALSE|NO_CONFIDENCE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fatal[TRUE|FALSE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cladeSampled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> specificEpithet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> infraspecificEpithet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lifeStage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dateIdentified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decimalLatitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decimalLongitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Collector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +93,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -67,15 +410,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,15 +886,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,32 +910,86 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O2" s="1">
+        <v>42315</v>
+      </c>
+      <c r="P2">
         <v>37</v>
       </c>
-      <c r="B2">
+      <c r="Q2">
         <v>-122</v>
       </c>
-      <c r="C2">
+      <c r="R2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="S2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O3" s="1">
+        <v>42323</v>
+      </c>
+      <c r="P3">
         <v>37.5</v>
       </c>
-      <c r="B3">
+      <c r="Q3">
         <v>-122</v>
       </c>
-      <c r="C3">
+      <c r="R3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="S3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more representative data file
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345"/>
   </bookViews>
   <sheets>
-    <sheet name="data-fims" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>collectionID</t>
   </si>
@@ -42,12 +42,6 @@
     <t xml:space="preserve"> sampleDisposition</t>
   </si>
   <si>
-    <t xml:space="preserve"> diseaseDetected[TRUE|FALSE|NO_CONFIDENCE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fatal[TRUE|FALSE]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cladeSampled</t>
   </si>
   <si>
@@ -79,6 +73,48 @@
   </si>
   <si>
     <t xml:space="preserve"> Collector</t>
+  </si>
+  <si>
+    <t>stuff</t>
+  </si>
+  <si>
+    <t>things</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>say</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fatal</t>
+  </si>
+  <si>
+    <t>your</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>ssp</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>plk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> diseaseDetected</t>
   </si>
 </sst>
 </file>
@@ -889,7 +925,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,46 +956,88 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
       <c r="O2" s="1">
         <v>42315</v>
       </c>
@@ -975,8 +1053,47 @@
       <c r="S2">
         <v>1</v>
       </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
       <c r="O3" s="1">
         <v>42323</v>
       </c>
@@ -991,6 +1108,9 @@
       </c>
       <c r="S3">
         <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update geo with more relevant examples
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>collectionID</t>
   </si>
@@ -115,6 +115,39 @@
   </si>
   <si>
     <t xml:space="preserve"> diseaseDetected</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <t>plktest</t>
+  </si>
+  <si>
+    <t>PLK3</t>
+  </si>
+  <si>
+    <t>B. d.</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Swab</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>NO_CONFIDENCE</t>
+  </si>
+  <si>
+    <t>plethodontidae</t>
+  </si>
+  <si>
+    <t>Batrachoseps</t>
+  </si>
+  <si>
+    <t>attenuatus</t>
   </si>
 </sst>
 </file>
@@ -922,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,8 +1109,8 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
+      <c r="H3" t="s">
+        <v>32</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -1110,6 +1143,65 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="1">
+        <v>42326</v>
+      </c>
+      <c r="P4">
+        <v>37.878086000000003</v>
+      </c>
+      <c r="Q4">
+        <v>-122.290059</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change some parsing after successful tests
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9350"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>collectionID</t>
   </si>
@@ -75,39 +75,9 @@
     <t xml:space="preserve"> Collector</t>
   </si>
   <si>
-    <t>stuff</t>
-  </si>
-  <si>
-    <t>things</t>
-  </si>
-  <si>
-    <t>have</t>
-  </si>
-  <si>
-    <t>you</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>say</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
     <t xml:space="preserve"> fatal</t>
   </si>
   <si>
-    <t>your</t>
-  </si>
-  <si>
-    <t>self</t>
-  </si>
-  <si>
-    <t>ssp</t>
-  </si>
-  <si>
     <t>adult</t>
   </si>
   <si>
@@ -117,9 +87,6 @@
     <t xml:space="preserve"> diseaseDetected</t>
   </si>
   <si>
-    <t>foobar</t>
-  </si>
-  <si>
     <t>plktest</t>
   </si>
   <si>
@@ -148,6 +115,15 @@
   </si>
   <si>
     <t>attenuatus</t>
+  </si>
+  <si>
+    <t>PLK1</t>
+  </si>
+  <si>
+    <t>PLK2</t>
+  </si>
+  <si>
+    <t>dendrobatidis</t>
   </si>
 </sst>
 </file>
@@ -958,15 +934,15 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -989,10 +965,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -1028,163 +1004,163 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1">
+        <v>42326</v>
+      </c>
+      <c r="P2">
+        <v>37.878086000000003</v>
+      </c>
+      <c r="Q2">
+        <v>-122.290059</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1">
-        <v>42315</v>
-      </c>
-      <c r="P2">
-        <v>37</v>
-      </c>
-      <c r="Q2">
-        <v>-122</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="H3" t="b">
         <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O3" s="1">
-        <v>42323</v>
+        <v>42326</v>
       </c>
       <c r="P3">
-        <v>37.5</v>
+        <v>37.878086000000003</v>
       </c>
       <c r="Q3">
-        <v>-122</v>
+        <v>-122.290059</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O4" s="1">
         <v>42326</v>
@@ -1202,7 +1178,7 @@
         <v>5</v>
       </c>
       <c r="T4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change defaults for more varied info in sample
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -934,7 +934,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,10 +1048,10 @@
         <v>42326</v>
       </c>
       <c r="P2">
-        <v>37.878086000000003</v>
+        <v>37.877000000000002</v>
       </c>
       <c r="Q2">
-        <v>-122.290059</v>
+        <v>-122.289</v>
       </c>
       <c r="R2">
         <v>3</v>
@@ -1166,10 +1166,10 @@
         <v>42326</v>
       </c>
       <c r="P4">
-        <v>37.878086000000003</v>
+        <v>37.878511000000003</v>
       </c>
       <c r="Q4">
-        <v>-122.290059</v>
+        <v>-122.288033</v>
       </c>
       <c r="R4">
         <v>3</v>

</xml_diff>

<commit_message>
Project upload feedback (Fixes #23)
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Worksheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>collectionID</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>dendrobatidis</t>
+  </si>
+  <si>
+    <t>Batrachochytridium dendrobatidus</t>
   </si>
 </sst>
 </file>
@@ -934,7 +937,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1015,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Fix never being able to validate
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -19,89 +19,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
   <si>
     <t>collectionID</t>
   </si>
   <si>
-    <t xml:space="preserve"> catalogNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fieldNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> diseaseTested</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> diseaseStrain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sampleMethod</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sampleDisposition</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cladeSampled</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> genus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> specificEpithet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> infraspecificEpithet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lifeStage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dateIdentified</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> decimalLatitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> decimalLongitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> coordinateUncertaintyInMeters</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fatal</t>
-  </si>
-  <si>
     <t>adult</t>
   </si>
   <si>
     <t>plk</t>
   </si>
   <si>
-    <t xml:space="preserve"> diseaseDetected</t>
-  </si>
-  <si>
     <t>plktest</t>
   </si>
   <si>
     <t>PLK3</t>
   </si>
   <si>
-    <t>B. d.</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>Swab</t>
-  </si>
-  <si>
     <t>Release</t>
   </si>
   <si>
@@ -126,9 +63,6 @@
     <t>dendrobatidis</t>
   </si>
   <si>
-    <t>Batrachochytridium dendrobatidus</t>
-  </si>
-  <si>
     <t>PLK4</t>
   </si>
   <si>
@@ -169,6 +103,72 @@
   </si>
   <si>
     <t>major</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>sampleType</t>
+  </si>
+  <si>
+    <t>Collector</t>
+  </si>
+  <si>
+    <t>decimalLongitude</t>
+  </si>
+  <si>
+    <t>decimalLatitude</t>
+  </si>
+  <si>
+    <t>lifeStage</t>
+  </si>
+  <si>
+    <t>coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t>infraspecificEpithet</t>
+  </si>
+  <si>
+    <t>specificEpithet</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>cladeSampled</t>
+  </si>
+  <si>
+    <t>fatal</t>
+  </si>
+  <si>
+    <t>diseaseDetected</t>
+  </si>
+  <si>
+    <t>sampleDisposition</t>
+  </si>
+  <si>
+    <t>diseaseStrain</t>
+  </si>
+  <si>
+    <t>diseaseTested</t>
+  </si>
+  <si>
+    <t>fieldNumber</t>
+  </si>
+  <si>
+    <t>catalogNumber</t>
+  </si>
+  <si>
+    <t>external Swab</t>
+  </si>
+  <si>
+    <t>dateCollected</t>
+  </si>
+  <si>
+    <t>Bd</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1024,107 +1024,110 @@
     <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1">
         <v>42326</v>
@@ -1142,30 +1145,33 @@
         <v>5</v>
       </c>
       <c r="T2" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -1174,16 +1180,16 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O3" s="1">
         <v>42326</v>
@@ -1201,48 +1207,51 @@
         <v>5</v>
       </c>
       <c r="T3" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1">
         <v>42326</v>
@@ -1260,30 +1269,33 @@
         <v>5</v>
       </c>
       <c r="T4" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1292,16 +1304,16 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1">
         <v>42383</v>
@@ -1319,30 +1331,33 @@
         <v>5</v>
       </c>
       <c r="T5" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U5" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -1351,16 +1366,16 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1">
         <v>42383</v>
@@ -1378,30 +1393,33 @@
         <v>5</v>
       </c>
       <c r="T6" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U6" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -1410,16 +1428,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="K7" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="N7" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1">
         <v>42383</v>
@@ -1437,30 +1455,33 @@
         <v>5</v>
       </c>
       <c r="T7" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U7" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
         <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1469,16 +1490,16 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O8" s="1">
         <v>42402</v>
@@ -1496,30 +1517,33 @@
         <v>5</v>
       </c>
       <c r="T8" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U8" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
         <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1528,16 +1552,16 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="L9" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O9" s="1">
         <v>42402</v>
@@ -1555,30 +1579,33 @@
         <v>5</v>
       </c>
       <c r="T9" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U9" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
         <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1587,16 +1614,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="O10" s="1">
         <v>42402</v>
@@ -1614,10 +1641,14 @@
         <v>5</v>
       </c>
       <c r="T10" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="U10" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix ark row and offline
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
   <si>
     <t>collectionID</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Bd</t>
+  </si>
+  <si>
+    <t>Dicamptodon</t>
+  </si>
+  <si>
+    <t>tenebrosus</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1019,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1307,10 +1313,10 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="L5" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="N5" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Try to trace why upload is being weird
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
   <si>
     <t>collectionID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>PLK8</t>
   </si>
   <si>
-    <t>PLK9</t>
-  </si>
-  <si>
     <t>Bufo</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>deprecated</t>
   </si>
   <si>
-    <t>Atelopus</t>
-  </si>
-  <si>
-    <t>rugulosus</t>
-  </si>
-  <si>
     <t>major</t>
   </si>
   <si>
@@ -175,6 +166,9 @@
   </si>
   <si>
     <t>tenebrosus</t>
+  </si>
+  <si>
+    <t>PLK30</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1013,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1035,64 +1029,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>35</v>
-      </c>
       <c r="T1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -1106,13 +1100,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1168,13 +1162,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -1230,13 +1224,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1292,13 +1286,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1313,10 +1307,10 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N5" t="s">
         <v>1</v>
@@ -1354,13 +1348,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1416,13 +1410,13 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1478,13 +1472,13 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -1496,13 +1490,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
         <v>20</v>
-      </c>
-      <c r="L8" t="s">
-        <v>21</v>
       </c>
       <c r="N8" t="s">
         <v>1</v>
@@ -1540,13 +1534,13 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1558,13 +1552,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s">
         <v>9</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
         <v>1</v>
@@ -1596,19 +1590,19 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -1620,13 +1614,13 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="N10" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Try to debug iffy saves
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="1">
-        <v>42402</v>
+        <v>42450</v>
       </c>
       <c r="P10">
         <v>37.886499999999998</v>

</xml_diff>

<commit_message>
Provide potential HTML feedback
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
   <si>
     <t>collectionID</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>tricolor</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <t>Psychrophrynella</t>
+  </si>
+  <si>
+    <t>chirihampatu</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1028,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="N6" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
For test uploads scoot up points
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -1028,18 +1028,18 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="P3" sqref="P2:P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>42326</v>
       </c>
       <c r="P2">
-        <v>37.877000000000002</v>
+        <v>38.877000000000002</v>
       </c>
       <c r="Q2">
         <v>-122.289</v>
@@ -1166,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>42326</v>
       </c>
       <c r="P3">
-        <v>37.878086000000003</v>
+        <v>38.878086000000003</v>
       </c>
       <c r="Q3">
         <v>-122.290059</v>
@@ -1228,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>42326</v>
       </c>
       <c r="P4">
-        <v>37.878511000000003</v>
+        <v>38.878511000000003</v>
       </c>
       <c r="Q4">
         <v>-122.288033</v>
@@ -1290,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>42383</v>
       </c>
       <c r="P5">
-        <v>37.880000000000003</v>
+        <v>38.880000000000003</v>
       </c>
       <c r="Q5">
         <v>-122.295</v>
@@ -1352,7 +1352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>42383</v>
       </c>
       <c r="P6">
-        <v>37.880000000000003</v>
+        <v>38.880000000000003</v>
       </c>
       <c r="Q6">
         <v>-122.28100000000001</v>
@@ -1414,7 +1414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>42383</v>
       </c>
       <c r="P7">
-        <v>37.869999999999997</v>
+        <v>38.869999999999997</v>
       </c>
       <c r="Q7">
         <v>-122.2894</v>
@@ -1476,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -1520,7 +1520,7 @@
         <v>42402</v>
       </c>
       <c r="P8">
-        <v>37.86</v>
+        <v>38.86</v>
       </c>
       <c r="Q8">
         <v>-122.3</v>
@@ -1538,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>42402</v>
       </c>
       <c r="P9">
-        <v>37.89</v>
+        <v>38.89</v>
       </c>
       <c r="Q9">
         <v>-122.27500000000001</v>
@@ -1600,7 +1600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>42450</v>
       </c>
       <c r="P10">
-        <v>37.886499999999998</v>
+        <v>38.886499999999998</v>
       </c>
       <c r="Q10">
         <v>-122.285</v>

</xml_diff>

<commit_message>
Attempt to fix decoding issues
</commit_message>
<xml_diff>
--- a/meta/geo.xlsx
+++ b/meta/geo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -147,9 +147,6 @@
     <t>diseaseTested</t>
   </si>
   <si>
-    <t>fieldNumber</t>
-  </si>
-  <si>
     <t>catalogNumber</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>chirihampatu</t>
+  </si>
+  <si>
+    <t>sampleID</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P2:P10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -1083,7 +1083,7 @@
         <v>31</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P1" t="s">
         <v>30</v>
@@ -1115,13 +1115,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1177,13 +1177,13 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -1198,10 +1198,10 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
         <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>51</v>
       </c>
       <c r="N3" t="s">
         <v>1</v>
@@ -1239,13 +1239,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1301,13 +1301,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1322,10 +1322,10 @@
         <v>8</v>
       </c>
       <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
         <v>47</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
       </c>
       <c r="N5" t="s">
         <v>1</v>
@@ -1363,13 +1363,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1381,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>53</v>
-      </c>
-      <c r="L6" t="s">
-        <v>54</v>
       </c>
       <c r="N6" t="s">
         <v>1</v>
@@ -1425,13 +1425,13 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1487,13 +1487,13 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -1549,13 +1549,13 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1605,19 +1605,19 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -1632,10 +1632,10 @@
         <v>23</v>
       </c>
       <c r="K10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" t="s">
         <v>47</v>
-      </c>
-      <c r="L10" t="s">
-        <v>48</v>
       </c>
       <c r="N10" t="s">
         <v>1</v>

</xml_diff>